<commit_message>
add new features in utils
</commit_message>
<xml_diff>
--- a/files/users.xlsx
+++ b/files/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\university-app\bot\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB7B3B0-E2C1-46CB-B461-CC3CF31E0E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505C6334-FB95-44D7-A0FC-7FABB7C8AC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18780" yWindow="4995" windowWidth="15900" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,19 +25,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Имя пользователя</t>
   </si>
   <si>
     <t>ID пользователя</t>
   </si>
+  <si>
+    <t>Ник пользователя</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,13 +48,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,7 +83,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -349,24 +364,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="1" max="3" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data in xlsx
</commit_message>
<xml_diff>
--- a/files/users.xlsx
+++ b/files/users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\university-app\bot\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505C6334-FB95-44D7-A0FC-7FABB7C8AC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF877F2C-0F25-48FC-9C33-966C035007E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18780" yWindow="4995" windowWidth="15900" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15900" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Имя пользователя</t>
   </si>
@@ -34,6 +34,48 @@
   </si>
   <si>
     <t>Ник пользователя</t>
+  </si>
+  <si>
+    <t>Саша</t>
+  </si>
+  <si>
+    <t>slunka322</t>
+  </si>
+  <si>
+    <t>Ксюша🫧</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Andris</t>
+  </si>
+  <si>
+    <t>Родион</t>
+  </si>
+  <si>
+    <t>f¡dgy</t>
+  </si>
+  <si>
+    <t>@yaderon</t>
+  </si>
+  <si>
+    <t>@slunka322</t>
+  </si>
+  <si>
+    <t>@kssyusshh</t>
+  </si>
+  <si>
+    <t>@SpecCorvo</t>
+  </si>
+  <si>
+    <t>@Tut_dedus</t>
+  </si>
+  <si>
+    <t>@Nx1dxr</t>
+  </si>
+  <si>
+    <t>@fiidgy</t>
   </si>
 </sst>
 </file>
@@ -81,9 +123,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -364,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,6 +429,83 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>931591593</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>886229823</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1260079637</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5450675821</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>635469686</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1030349543</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1122159904</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>